<commit_message>
Update .xlsx template form.
</commit_message>
<xml_diff>
--- a/app/assets/images/forma_csv.xlsx
+++ b/app/assets/images/forma_csv.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="200" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,18 +115,6 @@
     <t>Dengue:  D        Chikungunya:  C</t>
   </si>
   <si>
-    <t>Ejemplo:  2C1D</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>(2 casos de chik y 1 caso de dengue)</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Permiso </t>
     </r>
@@ -149,6 +137,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Ejemplo: C(m20)D(f3,f010)</t>
+  </si>
+  <si>
+    <t>1 caso de Chikungunya, de sexo masculino, 20 años de edad; y 2 cases of dengue, ambas de sexo femenino, de 3 años y 10 meses de edad, respectivamente.</t>
   </si>
 </sst>
 </file>
@@ -551,6 +545,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -560,12 +556,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,9 +594,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -982,7 +976,7 @@
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="22"/>
@@ -990,12 +984,12 @@
       <c r="E2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="36"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="36"/>
+      <c r="I2" s="38"/>
       <c r="J2" s="17"/>
       <c r="K2" s="44" t="s">
         <v>20</v>
@@ -1012,11 +1006,11 @@
       </c>
       <c r="F3" s="56"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
       <c r="K3" s="46" t="s">
         <v>24</v>
       </c>
@@ -1032,17 +1026,17 @@
       </c>
       <c r="F4" s="56"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
       <c r="K4" s="46" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="L4" s="51"/>
     </row>
-    <row r="5" spans="1:13" ht="20" customHeight="1">
+    <row r="5" spans="1:13" ht="58" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -1050,17 +1044,17 @@
       <c r="E5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="40" t="s">
-        <v>26</v>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="59" t="s">
+        <v>31</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="60"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="C6" s="7"/>
@@ -1071,7 +1065,7 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -1084,29 +1078,29 @@
       <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
-      <c r="A8" s="38" t="s">
-        <v>30</v>
+      <c r="A8" s="40" t="s">
+        <v>28</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1">
-      <c r="A9" s="37" t="s">
-        <v>29</v>
+      <c r="A9" s="39" t="s">
+        <v>27</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
@@ -1429,8 +1423,8 @@
       <c r="L30" s="25"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A31" s="60" t="s">
-        <v>31</v>
+      <c r="A31" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="B31" s="26"/>
       <c r="C31" s="30"/>
@@ -5318,11 +5312,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
@@ -5332,9 +5321,14 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:G5"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Fix typo in csv template.
</commit_message>
<xml_diff>
--- a/app/assets/images/forma_csv.xlsx
+++ b/app/assets/images/forma_csv.xlsx
@@ -142,7 +142,7 @@
     <t>Ejemplo: C(m20)D(f3,f010)</t>
   </si>
   <si>
-    <t>1 caso de Chikungunya, de sexo masculino, 20 años de edad; y 2 cases of dengue, ambas de sexo femenino, de 3 años y 10 meses de edad, respectivamente.</t>
+    <t>1 caso de Chikungunya, de sexo masculino, 20 años de edad; y 2 casos de dengue, ambos de sexo femenino, de 3 años y 10 meses de edad, respectivamente.</t>
   </si>
 </sst>
 </file>
@@ -546,16 +546,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -591,16 +581,26 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,7 +935,7 @@
   <dimension ref="A1:M999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -958,21 +958,21 @@
       <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="52" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="14"/>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="43"/>
+      <c r="L1" s="37"/>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
       <c r="A2" s="15" t="s">
@@ -981,80 +981,80 @@
       <c r="B2" s="1"/>
       <c r="C2" s="22"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="38"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="38"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="44" t="s">
+      <c r="K2" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="45"/>
+      <c r="L2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="20" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="56"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="46" t="s">
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="47"/>
+      <c r="L3" s="41"/>
     </row>
     <row r="4" spans="1:13" ht="20" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="56"/>
+      <c r="F4" s="51"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="46" t="s">
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="51"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:13" ht="58" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36" t="s">
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="59" t="s">
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="60"/>
+      <c r="L5" s="59"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="C6" s="7"/>
@@ -1078,29 +1078,29 @@
       <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
@@ -5312,6 +5312,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
@@ -5323,12 +5329,6 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="E5:G5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>